<commit_message>
cleaned up valueset URLs, added Risk Assessment and Obs for HCC flags
</commit_message>
<xml_diff>
--- a/prototype/alr_ig/output/StructureDefinition-alr-Group.xlsx
+++ b/prototype/alr_ig/output/StructureDefinition-alr-Group.xlsx
@@ -128,7 +128,7 @@
     <t>Mapping: FiveWs Pattern Mapping</t>
   </si>
   <si>
-    <t>Mapping: Legacy CSV Assignment List Report</t>
+    <t>Mapping: CMS Assignment List Report</t>
   </si>
   <si>
     <t>Group</t>
@@ -1245,7 +1245,7 @@
     <t>ALR Change Reason Description</t>
   </si>
   <si>
-    <t>GHP_EXCLUDED</t>
+    <t>OTHER_SHARED_SAV_INT</t>
   </si>
   <si>
     <t>ext-claimsBasedAssignmentFlag</t>
@@ -1517,44 +1517,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.75390625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="33.7109375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="40.90625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.5" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="31.33203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="95.9140625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="91.81640625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="147.61328125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="58.3125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="25.328125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="43.0625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="35.3359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="138.56640625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="53.8359375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="24.4609375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="192.80859375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="33.046875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="43.8515625" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="182.2109375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="32.84375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="35.96875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
added mappings and examples for table 1-5 and 1-6
</commit_message>
<xml_diff>
--- a/prototype/alr_ig/output/StructureDefinition-alr-Group.xlsx
+++ b/prototype/alr_ig/output/StructureDefinition-alr-Group.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$97</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3273" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3307" uniqueCount="438">
   <si>
     <t>Path</t>
   </si>
@@ -159,7 +159,7 @@
     <t>Entity[determinerCode="GRP" or determinerCode="GRP_KIND"]</t>
   </si>
   <si>
-    <t>ALR Table 1-1</t>
+    <t>ALR Table 1-6</t>
   </si>
   <si>
     <t>Group.id</t>
@@ -1248,7 +1248,7 @@
     <t>ALR Change Reason Description</t>
   </si>
   <si>
-    <t>OTHER_SHARED_SAV_INT</t>
+    <t>NOFND_R06</t>
   </si>
   <si>
     <t>ext-claimsBasedAssignmentFlag</t>
@@ -1317,6 +1317,19 @@
   </si>
   <si>
     <t>IN_VA_MAX</t>
+  </si>
+  <si>
+    <t>ext-vaSelectionOnlyFlag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://alr.cms.gov/ig/StructureDefinition/ext-vaSelectionOnlyFlag}
+</t>
+  </si>
+  <si>
+    <t>ALR Voluntary Alignment Selection Only</t>
+  </si>
+  <si>
+    <t>VA_SELECTION_ONLY</t>
   </si>
   <si>
     <t>Group.member.modifierExtension</t>
@@ -1511,7 +1524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL96"/>
+  <dimension ref="A1:AL97"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -11510,45 +11523,43 @@
         <v>418</v>
       </c>
     </row>
-    <row r="93" hidden="true">
+    <row r="93">
       <c r="A93" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="B93" t="s" s="2">
         <v>419</v>
       </c>
-      <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
-        <v>332</v>
+        <v>39</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F93" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G93" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H93" t="s" s="2">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I93" t="s" s="2">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="J93" t="s" s="2">
-        <v>69</v>
+        <v>420</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>333</v>
+        <v>421</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="M93" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="N93" t="s" s="2">
-        <v>160</v>
-      </c>
+        <v>421</v>
+      </c>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
       <c r="O93" t="s" s="2">
         <v>39</v>
       </c>
@@ -11596,7 +11607,7 @@
         <v>39</v>
       </c>
       <c r="AE93" t="s" s="2">
-        <v>335</v>
+        <v>76</v>
       </c>
       <c r="AF93" t="s" s="2">
         <v>40</v>
@@ -11611,50 +11622,54 @@
         <v>77</v>
       </c>
       <c r="AJ93" t="s" s="2">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="AK93" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL93" t="s" s="2">
-        <v>39</v>
+        <v>422</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
-        <v>39</v>
+        <v>332</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F94" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H94" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="H94" t="s" s="2">
-        <v>39</v>
-      </c>
       <c r="I94" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="J94" t="s" s="2">
-        <v>421</v>
+        <v>69</v>
       </c>
       <c r="K94" t="s" s="2">
-        <v>422</v>
+        <v>333</v>
       </c>
       <c r="L94" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="M94" s="2"/>
-      <c r="N94" s="2"/>
+        <v>334</v>
+      </c>
+      <c r="M94" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="N94" t="s" s="2">
+        <v>160</v>
+      </c>
       <c r="O94" t="s" s="2">
         <v>39</v>
       </c>
@@ -11702,22 +11717,22 @@
         <v>39</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>420</v>
+        <v>335</v>
       </c>
       <c r="AF94" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="AG94" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AH94" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI94" t="s" s="2">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="AJ94" t="s" s="2">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="AK94" t="s" s="2">
         <v>39</v>
@@ -11736,7 +11751,7 @@
       </c>
       <c r="D95" s="2"/>
       <c r="E95" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F95" t="s" s="2">
         <v>49</v>
@@ -11751,24 +11766,20 @@
         <v>39</v>
       </c>
       <c r="J95" t="s" s="2">
-        <v>261</v>
+        <v>425</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="M95" s="2"/>
-      <c r="N95" t="s" s="2">
-        <v>427</v>
-      </c>
+      <c r="N95" s="2"/>
       <c r="O95" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="P95" t="s" s="2">
-        <v>428</v>
-      </c>
+      <c r="P95" s="2"/>
       <c r="Q95" t="s" s="2">
         <v>39</v>
       </c>
@@ -11815,7 +11826,7 @@
         <v>424</v>
       </c>
       <c r="AF95" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="AG95" t="s" s="2">
         <v>49</v>
@@ -11838,7 +11849,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -11861,24 +11872,24 @@
         <v>39</v>
       </c>
       <c r="J96" t="s" s="2">
-        <v>231</v>
+        <v>261</v>
       </c>
       <c r="K96" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="L96" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="L96" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="M96" s="2"/>
       <c r="N96" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="O96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P96" t="s" s="2">
         <v>432</v>
       </c>
-      <c r="O96" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P96" t="s" s="2">
-        <v>433</v>
-      </c>
       <c r="Q96" t="s" s="2">
         <v>39</v>
       </c>
@@ -11922,7 +11933,7 @@
         <v>39</v>
       </c>
       <c r="AE96" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AF96" t="s" s="2">
         <v>40</v>
@@ -11946,8 +11957,118 @@
         <v>39</v>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="B97" s="2"/>
+      <c r="C97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F97" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="G97" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="H97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J97" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="K97" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="L97" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="M97" s="2"/>
+      <c r="N97" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="O97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P97" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="Q97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE97" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="AF97" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG97" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI97" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="AJ97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL97" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AL96">
+  <autoFilter ref="A1:AL97">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -11957,7 +12078,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI95">
+  <conditionalFormatting sqref="A2:AI96">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
mods based on Colin feedback - partDMonths extension and VA providers
</commit_message>
<xml_diff>
--- a/prototype/alr_ig/output/StructureDefinition-alr-Group.xlsx
+++ b/prototype/alr_ig/output/StructureDefinition-alr-Group.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$98</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3307" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3341" uniqueCount="441">
   <si>
     <t>Path</t>
   </si>
@@ -1317,6 +1317,16 @@
   </si>
   <si>
     <t>IN_VA_MAX</t>
+  </si>
+  <si>
+    <t>ext-voluntaryAlignmentProvider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://alr.cms.gov/ig/StructureDefinition/ext-voluntaryAlignmentProvider}
+</t>
+  </si>
+  <si>
+    <t>ALR Voluntary Alignment Provider</t>
   </si>
   <si>
     <t>ext-vaSelectionOnlyFlag</t>
@@ -1524,7 +1534,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL97"/>
+  <dimension ref="A1:AL98"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -11538,7 +11548,7 @@
         <v>40</v>
       </c>
       <c r="F93" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G93" t="s" s="2">
         <v>50</v>
@@ -11628,48 +11638,46 @@
         <v>39</v>
       </c>
       <c r="AL93" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="B94" t="s" s="2">
         <v>422</v>
       </c>
-    </row>
-    <row r="94" hidden="true">
-      <c r="A94" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
-        <v>332</v>
+        <v>39</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F94" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G94" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H94" t="s" s="2">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I94" t="s" s="2">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="J94" t="s" s="2">
-        <v>69</v>
+        <v>423</v>
       </c>
       <c r="K94" t="s" s="2">
-        <v>333</v>
+        <v>424</v>
       </c>
       <c r="L94" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="M94" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="N94" t="s" s="2">
-        <v>160</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
       <c r="O94" t="s" s="2">
         <v>39</v>
       </c>
@@ -11717,7 +11725,7 @@
         <v>39</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>335</v>
+        <v>76</v>
       </c>
       <c r="AF94" t="s" s="2">
         <v>40</v>
@@ -11732,50 +11740,54 @@
         <v>77</v>
       </c>
       <c r="AJ94" t="s" s="2">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="AK94" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL94" t="s" s="2">
-        <v>39</v>
+        <v>425</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
-        <v>39</v>
+        <v>332</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F95" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H95" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="H95" t="s" s="2">
-        <v>39</v>
-      </c>
       <c r="I95" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="J95" t="s" s="2">
-        <v>425</v>
+        <v>69</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>426</v>
+        <v>333</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="M95" s="2"/>
-      <c r="N95" s="2"/>
+        <v>334</v>
+      </c>
+      <c r="M95" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="N95" t="s" s="2">
+        <v>160</v>
+      </c>
       <c r="O95" t="s" s="2">
         <v>39</v>
       </c>
@@ -11823,22 +11835,22 @@
         <v>39</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>424</v>
+        <v>335</v>
       </c>
       <c r="AF95" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="AG95" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AH95" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI95" t="s" s="2">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="AJ95" t="s" s="2">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="AK95" t="s" s="2">
         <v>39</v>
@@ -11849,7 +11861,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -11857,7 +11869,7 @@
       </c>
       <c r="D96" s="2"/>
       <c r="E96" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F96" t="s" s="2">
         <v>49</v>
@@ -11872,7 +11884,7 @@
         <v>39</v>
       </c>
       <c r="J96" t="s" s="2">
-        <v>261</v>
+        <v>428</v>
       </c>
       <c r="K96" t="s" s="2">
         <v>429</v>
@@ -11881,15 +11893,11 @@
         <v>430</v>
       </c>
       <c r="M96" s="2"/>
-      <c r="N96" t="s" s="2">
-        <v>431</v>
-      </c>
+      <c r="N96" s="2"/>
       <c r="O96" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="P96" t="s" s="2">
-        <v>432</v>
-      </c>
+      <c r="P96" s="2"/>
       <c r="Q96" t="s" s="2">
         <v>39</v>
       </c>
@@ -11933,10 +11941,10 @@
         <v>39</v>
       </c>
       <c r="AE96" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AF96" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="AG96" t="s" s="2">
         <v>49</v>
@@ -11959,7 +11967,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="2">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -11982,23 +11990,23 @@
         <v>39</v>
       </c>
       <c r="J97" t="s" s="2">
-        <v>231</v>
+        <v>261</v>
       </c>
       <c r="K97" t="s" s="2">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="M97" s="2"/>
       <c r="N97" t="s" s="2">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="O97" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P97" t="s" s="2">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="Q97" t="s" s="2">
         <v>39</v>
@@ -12043,7 +12051,7 @@
         <v>39</v>
       </c>
       <c r="AE97" t="s" s="2">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="AF97" t="s" s="2">
         <v>40</v>
@@ -12067,8 +12075,118 @@
         <v>39</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="B98" s="2"/>
+      <c r="C98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F98" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="G98" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="H98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J98" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="K98" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="L98" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="M98" s="2"/>
+      <c r="N98" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="O98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P98" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="Q98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE98" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="AF98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG98" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI98" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="AJ98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL98" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AL97">
+  <autoFilter ref="A1:AL98">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -12078,7 +12196,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI96">
+  <conditionalFormatting sqref="A2:AI97">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>